<commit_message>
Add rechargeable battery options
</commit_message>
<xml_diff>
--- a/Cycle_Two/Scoring_Battery.xlsx
+++ b/Cycle_Two/Scoring_Battery.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="480" windowWidth="23960" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="460" yWindow="480" windowWidth="24180" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>MediCall</t>
   </si>
@@ -59,9 +59,6 @@
     <t>AA battery</t>
   </si>
   <si>
-    <t>Lithium-ion rechargeable battery</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
@@ -87,13 +84,92 @@
   </si>
   <si>
     <t>Weighted score (1-5)</t>
+  </si>
+  <si>
+    <t>Rechargeable AA battery</t>
+  </si>
+  <si>
+    <t>Among options of AA rechargeable batteries:</t>
+  </si>
+  <si>
+    <t>Panasonic Eneloop Pro</t>
+  </si>
+  <si>
+    <t>AmazonBasics High Capacity</t>
+  </si>
+  <si>
+    <t>Duracell Rechargeable</t>
+  </si>
+  <si>
+    <t>AmazonBasics Rechargeable Batteries</t>
+  </si>
+  <si>
+    <t>Energizer Recharge Universal</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Capacity (mAh)</t>
+  </si>
+  <si>
+    <t>Charging limit (times)</t>
+  </si>
+  <si>
+    <t>Cheapest market price/unit ($)</t>
+  </si>
+  <si>
+    <t>Runtime on one charge</t>
+  </si>
+  <si>
+    <t>9 hr 33 min</t>
+  </si>
+  <si>
+    <t>10 hr 45 min</t>
+  </si>
+  <si>
+    <t>9 hr 45 min</t>
+  </si>
+  <si>
+    <t>8 hr 20 min</t>
+  </si>
+  <si>
+    <t>8 hr 17 min</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>Charging cycle limit</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,6 +209,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -160,7 +244,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -197,29 +281,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -495,18 +600,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="K24" sqref="G18:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -552,36 +659,36 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>11</v>
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="10">
+        <v>1</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="12">
         <v>1</v>
       </c>
       <c r="E6" s="2">
@@ -591,16 +698,16 @@
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10">
         <v>2</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="C7" s="2">
         <v>-1</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="12">
         <v>1</v>
       </c>
       <c r="E7" s="2">
@@ -610,16 +717,16 @@
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="12">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="10">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="C8" s="2">
         <v>1</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="12">
         <v>1</v>
       </c>
       <c r="E8" s="2">
@@ -629,16 +736,16 @@
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="12">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="10">
         <v>4</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="C9" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="12">
         <v>1</v>
       </c>
       <c r="E9" s="2">
@@ -648,16 +755,16 @@
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="12">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="10">
         <v>3</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="C10" s="2">
         <v>-1</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="12">
         <v>-1</v>
       </c>
       <c r="E10" s="2">
@@ -667,16 +774,16 @@
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="13">
-        <v>1</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>17</v>
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="14">
+        <v>1</v>
       </c>
       <c r="C11" s="6">
         <v>1</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="13">
         <v>1</v>
       </c>
       <c r="E11" s="6">
@@ -686,14 +793,13 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="2">
         <v>4</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="12">
         <v>5</v>
       </c>
       <c r="E12" s="2">
@@ -703,14 +809,13 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="2">
         <v>-2</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="12">
         <v>-1</v>
       </c>
       <c r="E13" s="2">
@@ -720,14 +825,13 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="2">
         <v>2</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="12">
         <v>4</v>
       </c>
       <c r="E14" s="2">
@@ -737,24 +841,245 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="2">
-        <f>C6*$A$6+C7*$A$7+C8*$A$8+C9*$A$9+C10*$A$10+C11*$A$11</f>
+        <f>C6*$B$6+C7*$B$7+C8*$B$8+C9*$B$9+C10*$B$10+C11*$B$11</f>
         <v>6</v>
       </c>
-      <c r="D15" s="14">
-        <f>D6*$A$6+D7*$A$7+D8*$A$8+D9*$A$9+D10*$A$10+D11*$A$11</f>
+      <c r="D15" s="12">
+        <f>D6*$B$6+D7*$B$7+D8*$B$8+D9*$B$9+D10*$B$10+D11*$B$11</f>
         <v>10</v>
       </c>
       <c r="E15" s="2">
-        <f>E6*$A$6+E7*$A$7+E8*$A$8+E9*$A$9+E10*$A$10+E11*$A$11</f>
+        <f>E6*$B$6+E7*$B$7+E8*$B$8+E9*$B$9+E10*$B$10+E11*$B$11</f>
         <v>-6</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="18">
+        <f>26.3/4</f>
+        <v>6.5750000000000002</v>
+      </c>
+      <c r="C19">
+        <v>2550</v>
+      </c>
+      <c r="D19">
+        <v>500</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19" s="20">
+        <v>5</v>
+      </c>
+      <c r="K19">
+        <f>SUM(G19:J19)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="23">
+        <f>14.99/8</f>
+        <v>1.87375</v>
+      </c>
+      <c r="C20" s="21">
+        <v>2400</v>
+      </c>
+      <c r="D20" s="21">
+        <v>500</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="21">
+        <v>5</v>
+      </c>
+      <c r="H20" s="21">
+        <v>3</v>
+      </c>
+      <c r="I20" s="21">
+        <v>4</v>
+      </c>
+      <c r="J20" s="22">
+        <v>4</v>
+      </c>
+      <c r="K20" s="21">
+        <f t="shared" ref="K20:K23" si="0">SUM(G20:J20)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="18">
+        <f>14.48/4</f>
+        <v>3.62</v>
+      </c>
+      <c r="C21">
+        <v>2450</v>
+      </c>
+      <c r="D21">
+        <v>400</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21" s="20">
+        <v>3</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="18">
+        <f>9.27/4</f>
+        <v>2.3174999999999999</v>
+      </c>
+      <c r="C22">
+        <v>2000</v>
+      </c>
+      <c r="D22">
+        <v>1000</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>5</v>
+      </c>
+      <c r="J22" s="20">
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="18">
+        <f>9.99/5</f>
+        <v>1.998</v>
+      </c>
+      <c r="C23">
+        <v>2000</v>
+      </c>
+      <c r="D23">
+        <v>1000</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23" s="20">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C28" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>